<commit_message>
feat: status no campeonato
adicionado novos dados do time
</commit_message>
<xml_diff>
--- a/data/times_brasileirao_2023.xlsx
+++ b/data/times_brasileirao_2023.xlsx
@@ -22,19 +22,19 @@
     <t>Sigla</t>
   </si>
   <si>
+    <t>Atlético-MG</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>Athletico-PR</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
     <t>América-MG</t>
-  </si>
-  <si>
-    <t>CAM</t>
-  </si>
-  <si>
-    <t>Athletico-PR</t>
-  </si>
-  <si>
-    <t>CAP</t>
-  </si>
-  <si>
-    <t>Atlético-MG</t>
   </si>
   <si>
     <t>AME</t>
@@ -205,7 +205,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>